<commit_message>
Se libera version 1.1.0 de PC y 1.03 de PLC
</commit_message>
<xml_diff>
--- a/Historial/estructura paso.xlsx
+++ b/Historial/estructura paso.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hh\lavadora.net\Historial\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="211"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -213,7 +218,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -285,17 +290,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,6 +380,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -422,7 +430,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,7 +465,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,18 +691,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -783,30 +791,30 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="1"/>
       <c r="G8" s="3" t="s">
         <v>42</v>
@@ -825,11 +833,11 @@
       <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="1"/>
       <c r="G9" s="2" t="s">
         <v>58</v>
@@ -850,11 +858,11 @@
       <c r="A10" s="2">
         <v>2</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="G10" s="2" t="s">
         <v>25</v>
@@ -874,11 +882,11 @@
       <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="1"/>
       <c r="G11" s="2" t="s">
         <v>27</v>
@@ -898,11 +906,11 @@
       <c r="A12" s="2">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="G12" s="2" t="s">
         <v>29</v>
@@ -922,11 +930,11 @@
       <c r="A13" s="2">
         <v>5</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="1"/>
       <c r="G13" s="2" t="s">
         <v>31</v>
@@ -946,11 +954,11 @@
       <c r="A14" s="2">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="G14" s="2" t="s">
         <v>63</v>
@@ -970,11 +978,11 @@
       <c r="A15" s="2">
         <v>7</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="1"/>
       <c r="G15" s="2" t="s">
         <v>32</v>
@@ -994,11 +1002,11 @@
       <c r="A16" s="2">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="G16" s="2" t="s">
         <v>33</v>
@@ -1018,11 +1026,11 @@
       <c r="A17" s="2">
         <v>9</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2" t="s">
@@ -1043,11 +1051,11 @@
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="2" t="s">
@@ -1068,11 +1076,11 @@
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
@@ -1087,11 +1095,11 @@
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
@@ -1106,9 +1114,9 @@
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1120,9 +1128,9 @@
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1134,9 +1142,9 @@
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -1146,12 +1154,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
@@ -1160,11 +1167,12 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>